<commit_message>
Changed: Fix quantity of potentiometers.
</commit_message>
<xml_diff>
--- a/CPBO Nomenclature.xlsx
+++ b/CPBO Nomenclature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\favier\Nextcloud\Informatique\Projets\Control Panel BO\Dépôt GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Commun\Informatique\Projets\Control Panel BO\Dépôt GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6220CDFD-8CF9-40A6-A169-F4272A18104F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nomenclature" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Racailloux</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -152,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -386,15 +387,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Produits"/>
-    <tableColumn id="2" name="Référence"/>
-    <tableColumn id="3" name="Prix Unitaire" dataDxfId="3"/>
-    <tableColumn id="4" name="Quantité" dataDxfId="2"/>
-    <tableColumn id="6" name="Ports" dataDxfId="1"/>
-    <tableColumn id="5" name="Prix Total" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produits"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Référence"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prix Unitaire" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quantité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ports" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Prix Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,11 +697,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -981,14 +982,14 @@
         <v>0.55800000000000005</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="6">
         <v>0</v>
       </c>
       <c r="F13" s="6">
         <f>Tableau1[[#This Row],[Prix Unitaire]]*Tableau1[[#This Row],[Quantité]]+Tableau1[[#This Row],[Ports]]</f>
-        <v>0.55800000000000005</v>
+        <v>1.1160000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1212,29 +1213,29 @@
       </c>
       <c r="F29" s="12">
         <f>SUM(F2:F28)</f>
-        <v>123.31786666666669</v>
+        <v>123.87586666666668</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B4:B8" r:id="rId9" display="AliExpress"/>
-    <hyperlink ref="B21:B22" r:id="rId10" display="Aliexpress"/>
-    <hyperlink ref="B18" r:id="rId11"/>
-    <hyperlink ref="B23" r:id="rId12"/>
-    <hyperlink ref="B20" r:id="rId13"/>
-    <hyperlink ref="B26" r:id="rId14"/>
-    <hyperlink ref="B24" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B25" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B4:B8" r:id="rId9" display="AliExpress" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B21:B22" r:id="rId10" display="Aliexpress" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B24" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>

</xml_diff>